<commit_message>
added functionallaty to read in symbol table from excell
</commit_message>
<xml_diff>
--- a/I_O_info_plc/DBs_PLC_300.xlsx
+++ b/I_O_info_plc/DBs_PLC_300.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F385C6B-9F1E-4636-83A2-B2D7587D3D7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCD7C90-A7B6-4D4F-9E28-31010A846821}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="8064" activeTab="3" xr2:uid="{F0EA8FC1-244E-4AA3-8AE3-B5F573F69DD9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="8064" activeTab="4" xr2:uid="{F0EA8FC1-244E-4AA3-8AE3-B5F573F69DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="DB2" sheetId="1" r:id="rId1"/>
     <sheet name="DB1" sheetId="2" r:id="rId2"/>
     <sheet name="DB3" sheetId="3" r:id="rId3"/>
     <sheet name="info_PLC" sheetId="4" r:id="rId4"/>
-    <sheet name="READ_ME" sheetId="5" r:id="rId5"/>
+    <sheet name="Symbol_table" sheetId="6" r:id="rId5"/>
+    <sheet name="READ_ME" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
   <si>
     <t>DB_VAR</t>
   </si>
@@ -239,6 +240,33 @@
   </si>
   <si>
     <t>10.34.0.95</t>
+  </si>
+  <si>
+    <t>test_name</t>
+  </si>
+  <si>
+    <t>I       0.0</t>
+  </si>
+  <si>
+    <t>other name</t>
+  </si>
+  <si>
+    <t>I       0.1</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>Q       0.1</t>
+  </si>
+  <si>
+    <t>test comment</t>
   </si>
 </sst>
 </file>
@@ -598,7 +626,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054A1064-456F-4C59-ACD3-1F866938F211}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1107,6 +1135,71 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7420531A-EB5E-4033-8E03-478F91AB9D7D}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693EEB1F-2430-4777-BB31-48467266A2A4}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
added functionally to read an write inputs
</commit_message>
<xml_diff>
--- a/I_O_info_plc/DBs_PLC_300.xlsx
+++ b/I_O_info_plc/DBs_PLC_300.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCD7C90-A7B6-4D4F-9E28-31010A846821}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8BF22E-7370-41EE-B81F-977B148EFB14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="8064" activeTab="4" xr2:uid="{F0EA8FC1-244E-4AA3-8AE3-B5F573F69DD9}"/>
   </bookViews>
@@ -245,15 +245,9 @@
     <t>test_name</t>
   </si>
   <si>
-    <t>I       0.0</t>
-  </si>
-  <si>
     <t>other name</t>
   </si>
   <si>
-    <t>I       0.1</t>
-  </si>
-  <si>
     <t>Symbol</t>
   </si>
   <si>
@@ -263,10 +257,16 @@
     <t>out</t>
   </si>
   <si>
-    <t>Q       0.1</t>
-  </si>
-  <si>
     <t>test comment</t>
+  </si>
+  <si>
+    <t>Q       8.1</t>
+  </si>
+  <si>
+    <t>I       4.0</t>
+  </si>
+  <si>
+    <t>I       4.1</t>
   </si>
 </sst>
 </file>
@@ -1139,20 +1139,20 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1163,7 +1163,7 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1171,10 +1171,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1182,16 +1182,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>